<commit_message>
commiting  report ang logging with headless
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/TC_Canine_Filter_1.xlsx
+++ b/CTDC_Automation/TestData/TC_Canine_Filter_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\KatalonApril24\DataCommons_Automation\CTDC_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\KatalonUploading\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497A30C7-EE16-4EAC-8C38-BD0991F14EBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE3AC6D-422F-471D-A941-A3BC9BC8266D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="3105" windowWidth="12225" windowHeight="7815" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="2" r:id="rId1"/>
@@ -310,9 +310,6 @@
     <t>Select_case_checkbox</t>
   </si>
   <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WITH DISTINCT c AS c, p, s, demo, diag RETURN c.case_id AS `Case ID`, s.clinical_study_designation AS `Study Code`, s.clinical_study_type AS `Study Type`, demo.breed AS Breed, diag.disease_term AS Diagnosis, diag.stage_of_disease AS `Stage of Disease`,demo.patient_age_at_enrollment AS Age, demo.sex AS Sex, demo.neutered_indicator AS `Neutered Status`</t>
-  </si>
-  <si>
     <t>compare</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
     <t>G_rowcount</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description </t>
   </si>
   <si>
@@ -377,13 +371,20 @@
   </si>
   <si>
     <t>bolt://ncias-s2261-c.nci.nih.gov:7687</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WITH DISTINCT c AS c, p, s, demo, diag RETURN c.case_id AS `Case ID`, s.clinical_study_designation AS `Study Code`, s.clinical_study_type AS `Study Type`, demo.breed AS Breed, diag.disease_term AS Diagnosis, coalesce(diag.stage_of_disease,'') AS `Stage of Disease`,demo.patient_age_at_enrollment AS Age, demo.sex AS Sex, coalesce(demo.neutered_indicator,'') AS `Neutered Status`
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +406,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -429,11 +436,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -752,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C468257-9521-42A0-A4DB-E0691FA7FE45}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,6 +773,7 @@
     <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.7109375" customWidth="1"/>
     <col min="7" max="7" width="99.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -840,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -855,7 +866,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H3" t="s">
         <v>22</v>
@@ -925,7 +936,7 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
@@ -960,7 +971,7 @@
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -1018,11 +1029,11 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
         <v>97</v>
       </c>
-      <c r="D8" t="s">
-        <v>98</v>
-      </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
@@ -1030,7 +1041,7 @@
         <v>20</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -1080,7 +1091,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1105,8 +1116,8 @@
       <c r="H10" t="s">
         <v>20</v>
       </c>
-      <c r="I10" t="s">
-        <v>92</v>
+      <c r="I10" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="J10" t="s">
         <v>43</v>
@@ -1144,7 +1155,7 @@
         <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1176,45 +1187,45 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1224,13 +1235,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
         <v>111</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" t="s">
-        <v>113</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
@@ -1241,7 +1252,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
This is Katalon Branch
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/TC_Canine_Filter_1.xlsx
+++ b/CTDC_Automation/TestData/TC_Canine_Filter_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\KatalonUploading\DataCommons_Automation\CTDC_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Script\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE3AC6D-422F-471D-A941-A3BC9BC8266D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F5F8D2-A64C-41AE-ACF4-C85E2A148983}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="120">
   <si>
     <t>Browser</t>
   </si>
@@ -320,9 +320,6 @@
   </si>
   <si>
     <t>//div[ contains(text(),'Case')]//parent::span//parent::th//parent::tr//parent::thead//parent::table/thead</t>
-  </si>
-  <si>
-    <t>rowcount</t>
   </si>
   <si>
     <t>G_rowcount</t>
@@ -378,6 +375,24 @@
   <si>
     <t xml:space="preserve">MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WITH DISTINCT c AS c, p, s, demo, diag RETURN c.case_id AS `Case ID`, s.clinical_study_designation AS `Study Code`, s.clinical_study_type AS `Study Type`, demo.breed AS Breed, diag.disease_term AS Diagnosis, coalesce(diag.stage_of_disease,'') AS `Stage of Disease`,demo.patient_age_at_enrollment AS Age, demo.sex AS Sex, coalesce(demo.neutered_indicator,'') AS `Neutered Status`
 </t>
+  </si>
+  <si>
+    <t>Canine_Cases</t>
+  </si>
+  <si>
+    <t>Canine_CasesTable</t>
+  </si>
+  <si>
+    <t>Canine_TableBody</t>
+  </si>
+  <si>
+    <t>Canine_NextBtn</t>
+  </si>
+  <si>
+    <t>Canine_TableHeader</t>
+  </si>
+  <si>
+    <t>Canine_RowCount</t>
   </si>
 </sst>
 </file>
@@ -762,21 +777,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C468257-9521-42A0-A4DB-E0691FA7FE45}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="76" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="7" max="7" width="99.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.7265625" customWidth="1"/>
+    <col min="7" max="7" width="99.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -811,7 +826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -846,7 +861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -854,7 +869,7 @@
         <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -866,7 +881,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H3" t="s">
         <v>22</v>
@@ -881,7 +896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -889,7 +904,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
         <v>55</v>
@@ -916,7 +931,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -924,7 +939,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
         <v>59</v>
@@ -951,7 +966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -959,7 +974,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="D6" t="s">
         <v>57</v>
@@ -986,7 +1001,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -994,7 +1009,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
         <v>61</v>
@@ -1021,7 +1036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1029,11 +1044,11 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" t="s">
         <v>96</v>
       </c>
-      <c r="D8" t="s">
-        <v>97</v>
-      </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
@@ -1041,7 +1056,7 @@
         <v>20</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -1056,7 +1071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1091,7 +1106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="70.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1117,7 +1132,7 @@
         <v>20</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J10" t="s">
         <v>43</v>
@@ -1126,7 +1141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1176,72 +1191,72 @@
       <selection activeCell="B4" sqref="B4:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
         <v>98</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>106</v>
       </c>
-      <c r="B7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" t="s">
         <v>110</v>
-      </c>
-      <c r="C11" t="s">
-        <v>111</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
@@ -1250,47 +1265,47 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D28" t="s">
         <v>37</v>
       </c>
@@ -1298,12 +1313,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D31" t="s">
         <v>37</v>
       </c>
@@ -1311,27 +1326,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D39" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -1366,7 +1381,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -1401,7 +1416,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -1436,7 +1451,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1471,7 +1486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -1506,7 +1521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -1538,7 +1553,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -1573,7 +1588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -1608,7 +1623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -1643,7 +1658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1678,7 +1693,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -1713,7 +1728,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>20</v>
       </c>
@@ -1748,7 +1763,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -1783,7 +1798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -1818,7 +1833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -1853,7 +1868,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -1888,7 +1903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -1923,7 +1938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -1958,7 +1973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>1</v>
       </c>
@@ -1993,7 +2008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -2028,12 +2043,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C66" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C69" t="s">
         <v>77</v>
       </c>
@@ -2041,7 +2056,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C70" t="s">
         <v>71</v>
       </c>
@@ -2049,7 +2064,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C71" t="s">
         <v>80</v>
       </c>
@@ -2057,7 +2072,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C72" t="s">
         <v>82</v>
       </c>
@@ -2065,7 +2080,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C73" t="s">
         <v>74</v>
       </c>
@@ -2073,7 +2088,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C74" t="s">
         <v>84</v>
       </c>
@@ -2081,7 +2096,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C75" t="s">
         <v>86</v>
       </c>
@@ -2089,7 +2104,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -2124,7 +2139,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>1</v>
       </c>
@@ -2159,7 +2174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>1</v>
       </c>
@@ -2194,7 +2209,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>1</v>
       </c>
@@ -2229,7 +2244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -2264,7 +2279,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>20</v>
       </c>
@@ -2299,7 +2314,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>20</v>
       </c>
@@ -2334,7 +2349,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>20</v>
       </c>
@@ -2369,7 +2384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>20</v>
       </c>

</xml_diff>